<commit_message>
draft of equivalence testing
</commit_message>
<xml_diff>
--- a/data/clean/EVS_Data_Quality_Overview_v2.xlsx
+++ b/data/clean/EVS_Data_Quality_Overview_v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="448">
   <si>
     <t>v1</t>
   </si>
@@ -2983,10 +2983,10 @@
   <dimension ref="A1:L287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K60" sqref="K60"/>
+      <selection pane="bottomRight" activeCell="J149" sqref="J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,11 +3064,9 @@
         <v>1</v>
       </c>
       <c r="J2" s="32">
-        <v>1</v>
-      </c>
-      <c r="K2" s="40" t="s">
-        <v>421</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -3168,11 +3166,9 @@
         <v>1</v>
       </c>
       <c r="J6" s="32">
-        <v>1</v>
-      </c>
-      <c r="K6" s="40" t="s">
-        <v>421</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3197,11 +3193,9 @@
         <v>1</v>
       </c>
       <c r="J7" s="33">
-        <v>1</v>
-      </c>
-      <c r="K7" s="40" t="s">
-        <v>421</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -4383,8 +4377,8 @@
       <c r="B59" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>390</v>
+      <c r="C59" s="17">
+        <v>2</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -4397,7 +4391,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59" s="41" t="s">
         <v>447</v>
@@ -4410,8 +4404,8 @@
       <c r="B60" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>390</v>
+      <c r="C60" s="5">
+        <v>2</v>
       </c>
       <c r="H60" s="12">
         <v>1</v>
@@ -4420,7 +4414,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" s="41" t="s">
         <v>447</v>
@@ -4433,8 +4427,8 @@
       <c r="B61" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>390</v>
+      <c r="C61" s="5">
+        <v>2</v>
       </c>
       <c r="H61" s="12">
         <v>1</v>
@@ -4443,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" s="41" t="s">
         <v>447</v>
@@ -4456,8 +4450,8 @@
       <c r="B62" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>390</v>
+      <c r="C62" s="8">
+        <v>2</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -4470,7 +4464,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="41" t="s">
         <v>447</v>
@@ -6730,7 +6724,7 @@
         <v>1</v>
       </c>
       <c r="K149" s="40" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
@@ -10391,7 +10385,7 @@
       </c>
       <c r="J287" s="35">
         <f>SUBTOTAL(109,Tabelle1[Measurement Invariance])</f>
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="K287" s="39"/>
       <c r="L287" s="22" t="s">

</xml_diff>